<commit_message>
new API, new bot
</commit_message>
<xml_diff>
--- a/TEMPLATES.xlsx
+++ b/TEMPLATES.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ЭтаКнига" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RUShulpiAn\Desktop\ServiceBot\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RUShulpiAn.NESTLESOFT\Desktop\ServiceBot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99B0C8AF-AB65-425F-B2F3-A979952378D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59E6919B-A7FB-472D-A96D-B0648661BDA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{E5075ABA-72E7-4528-8386-FF76AF21FACD}"/>
+    <workbookView xWindow="-60" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{E5075ABA-72E7-4528-8386-FF76AF21FACD}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="83">
   <si>
     <t>Выдача оборудования и аксессуаров / Issuance of equipment and accessories · ELMA365</t>
   </si>
@@ -107,25 +107,13 @@
     <t>Для выдачи нового оборудования вам необходимо оформить обращение по ссылке:</t>
   </si>
   <si>
-    <t>Для получения SIM-карты и других манипуляций, касающихся мобильной связи, заполните заявку по ссылке:</t>
-  </si>
-  <si>
     <t>Для получения поддержки по программному обеспечению заполните заявку по ссылке:</t>
   </si>
   <si>
-    <t>Для передачи оборудования оформите заявку по ссылке:</t>
-  </si>
-  <si>
     <t>Для решения проблемы с IT-оборудованием обратитесь по ссылке:</t>
   </si>
   <si>
     <t>Для бронирования временного оборудования заполните заявку по ссылке:</t>
-  </si>
-  <si>
-    <t>Для организации поддержки мероприятия заполните заявку по ссылке:</t>
-  </si>
-  <si>
-    <t>Для обслуживания принтера заполните заявку по ссылке:</t>
   </si>
   <si>
     <t>Для получения доступа к Консультант Плюс оформите заявку по ссылке:</t>
@@ -272,20 +260,59 @@
     <t>Для запроса ролей в SAP Prod (R9*) заполните заявку ниже:</t>
   </si>
   <si>
-    <t>Для сброса пароля в Local SAP Prod (R9*) заполните заявку ниже:</t>
-  </si>
-  <si>
     <t>Для запроса ролей в SAP non-Prod (R5*, R8*) заполните заявку ниже:</t>
   </si>
   <si>
-    <t>Для сброса пароля в Local SAP non-Prod (R5*, R8*) заполните заявку ниже:</t>
+    <t>Приложите скриншот ошибки, пожалуйста.</t>
+  </si>
+  <si>
+    <t>Уточните номер заявки, пожалуйста.</t>
+  </si>
+  <si>
+    <t>Для передачи своего оборудования другому сотруднику оформите заявку по ссылке:</t>
+  </si>
+  <si>
+    <t>Для оказания поддержки на мероприятии заполните заявку по ссылке:</t>
+  </si>
+  <si>
+    <t>Для обслуживания принтера (только Московский офис) заполните заявку по ссылке:</t>
+  </si>
+  <si>
+    <t>Когда просят настроить Telegram/WhatsApp/...</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Чтобы изменить тип лицензии на вашей учетной записи оформите заявку ниже:  </t>
+  </si>
+  <si>
+    <t>Создание или изменение лицензии почтового ящика / Mailbox creation and O365 License change · ELMA365</t>
+  </si>
+  <si>
+    <t>https://elma.nestle.ru/_portal/service_desk/query_catalog(p:run/service_desk.applications/mailbox_creation_and_o365_license_change;values=%7B%7D)</t>
+  </si>
+  <si>
+    <t>Нет доступа к настольным приложениям Office 365</t>
+  </si>
+  <si>
+    <t>Использование некорпоративных мессенджеров в корпоративных целях запрещено.</t>
+  </si>
+  <si>
+    <t>Для получения/открепления/перевыпуска SIM-карты или изменения мобильных сервисов, заполните заявку по ссылке:</t>
+  </si>
+  <si>
+    <t>Поднимите данный запрос, если необходимо разработать новый ЗНО, доработать уже существующее решение на платформе ELMA365:</t>
+  </si>
+  <si>
+    <t>Для сброса пароля/разблокирования учетной записи в Local SAP Prod (R9*) заполните заявку ниже:</t>
+  </si>
+  <si>
+    <t>Для сброса пароля/разблокирования учетной записи в Local SAP non-Prod (R5*, R8*) заполните заявку ниже:</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -316,13 +343,45 @@
       <name val="Nestle Text TF Light"/>
       <charset val="204"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF94DCF8"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -338,11 +397,30 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -681,309 +759,353 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA025EF0-5A23-4366-8147-699F1C81AA69}">
   <sheetPr codeName="Лист1"/>
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="39.08984375" style="3" customWidth="1"/>
+    <col min="1" max="1" width="39.1796875" style="3" customWidth="1"/>
     <col min="2" max="2" width="90" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B1" t="s">
-        <v>50</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="B1" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="5" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="29.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="6" t="s">
         <v>22</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" t="s">
-        <v>51</v>
+      <c r="C2" s="5" t="s">
+        <v>47</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A3" s="3" t="s">
-        <v>23</v>
+      <c r="A3" s="7" t="s">
+        <v>79</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C3" t="s">
-        <v>52</v>
+      <c r="C3" s="5" t="s">
+        <v>48</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A4" s="3" t="s">
-        <v>24</v>
+      <c r="A4" s="6" t="s">
+        <v>23</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C4" t="s">
-        <v>53</v>
+      <c r="C4" s="5" t="s">
+        <v>49</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A5" s="3" t="s">
-        <v>69</v>
+      <c r="A5" s="6" t="s">
+        <v>65</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C5" t="s">
-        <v>54</v>
+      <c r="C5" s="5" t="s">
+        <v>50</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A6" s="3" t="s">
-        <v>25</v>
+      <c r="A6" s="7" t="s">
+        <v>70</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C6" t="s">
-        <v>55</v>
+      <c r="C6" s="5" t="s">
+        <v>51</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A7" s="3" t="s">
-        <v>26</v>
+      <c r="A7" s="6" t="s">
+        <v>24</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C7" t="s">
-        <v>56</v>
+      <c r="C7" s="5" t="s">
+        <v>52</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A8" s="3" t="s">
-        <v>27</v>
+      <c r="A8" s="6" t="s">
+        <v>25</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C8" t="s">
-        <v>57</v>
+      <c r="C8" s="5" t="s">
+        <v>53</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A9" s="3" t="s">
-        <v>28</v>
+      <c r="A9" s="7" t="s">
+        <v>71</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C9" t="s">
-        <v>58</v>
+      <c r="C9" s="5" t="s">
+        <v>54</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A10" s="3" t="s">
-        <v>29</v>
+    <row r="10" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A10" s="7" t="s">
+        <v>72</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C10" t="s">
-        <v>59</v>
+      <c r="C10" s="5" t="s">
+        <v>55</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A11" s="3" t="s">
-        <v>30</v>
+      <c r="A11" s="6" t="s">
+        <v>26</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="D11" s="5"/>
+    </row>
+    <row r="12" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A12" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A13" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A14" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="58" x14ac:dyDescent="0.35">
+      <c r="A15" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C15" s="5" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A12" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C12" t="s">
+      <c r="D15" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A16" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C16" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="D12" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A13" s="3" t="s">
+      <c r="D16" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A17" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="D17" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B13" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C13" t="s">
-        <v>62</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A14" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C14" t="s">
+    </row>
+    <row r="18" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A18" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C18" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="D14" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="58" x14ac:dyDescent="0.35">
-      <c r="A15" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C15" t="s">
+      <c r="D18" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A19" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C19" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="D15" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A16" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C16" t="s">
-        <v>65</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A17" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C17" t="s">
-        <v>66</v>
-      </c>
-      <c r="D17" s="2" t="s">
+      <c r="D19" s="2" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A18" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="C18" t="s">
-        <v>67</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A19" s="3" t="s">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A20" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="B20" s="5"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A21" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="B21" s="5"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+    </row>
+    <row r="22" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A22" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="B22" s="5"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="B19" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C19" t="s">
-        <v>68</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>49</v>
+    </row>
+    <row r="23" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A23" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="B23" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>77</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="https://elma.nestle.ru/_portal/service_desk/query_catalog(p:run/service_desk.applications/equipment_issuance;values=%7B%7D)" xr:uid="{3B2646A4-08BA-40BC-8AD8-6DEE2CD9C942}"/>
-    <hyperlink ref="B3" r:id="rId2" display="https://elma.nestle.ru/_portal/service_desk/query_catalog(p:run/service_desk.applications/mobile_service;values=%7B%7D)" xr:uid="{38610046-EA87-42D2-941F-CB3F40E05BE5}"/>
-    <hyperlink ref="B4" r:id="rId3" display="https://elma.nestle.ru/_portal/service_desk/query_catalog(p:run/service_desk.applications/software_maintenance;values=%7B%7D)" xr:uid="{00F691E7-D2E4-497A-8306-93843142617C}"/>
-    <hyperlink ref="B5" r:id="rId4" display="https://elma.nestle.ru/_portal/service_desk/query_catalog(p:run/service_desk.applications/installing_drivers_for_printers;values=%7B%7D)" xr:uid="{7B7CBB90-1C6C-4098-B654-B2ED53E0DCE3}"/>
-    <hyperlink ref="B6" r:id="rId5" display="https://elma.nestle.ru/_portal/service_desk/query_catalog(p:run/service_desk.applications/transfer_equipment;values=%7B%7D)" xr:uid="{B02B9564-D849-4003-B375-CD8C56721EC9}"/>
-    <hyperlink ref="B7" r:id="rId6" display="https://elma.nestle.ru/_portal/service_desk/query_catalog(p:run/service_desk.applications/IT_issue;values=%7B%7D)" xr:uid="{13DC51EB-B7C9-4DA7-A793-0AECE8A8B324}"/>
-    <hyperlink ref="B8" r:id="rId7" display="https://elma.nestle.ru/_portal/service_desk/query_catalog(p:run/service_desk.applications/booking_equipment;values=%7B%7D)" xr:uid="{93D588E9-77DB-4602-8C87-440DCEB6312D}"/>
-    <hyperlink ref="B9" r:id="rId8" display="https://elma.nestle.ru/_portal/service_desk/query_catalog(p:run/service_desk.applications/event_support;values=%7B%7D)" xr:uid="{266DAB29-E809-48CD-BE96-0F3E87029138}"/>
-    <hyperlink ref="B10" r:id="rId9" display="https://elma.nestle.ru/_portal/service_desk/query_catalog(p:run/service_desk.applications/Printer_maintenance;values=%7B%7D)" xr:uid="{11871A81-F344-4D2B-A0BB-312231FBFF37}"/>
-    <hyperlink ref="B11" r:id="rId10" display="https://elma.nestle.ru/_portal/service_desk/query_catalog(p:run/service_desk.applications/consultant_plus;values=%7B%7D)" xr:uid="{68D9DB9F-F34C-4AA1-B673-EC8F7DBBEA9D}"/>
-    <hyperlink ref="B12" r:id="rId11" display="https://eur02.safelinks.protection.outlook.com/?url=https%3A%2F%2Felma.nestle.ru%2F_portal%2Fservice_desk%2Fquery_catalog(p%3Arun%2Fservice_desk.applications%2Frobots_report_an_issue%3Bvalues%3D%257B%257D)&amp;data=05%7C02%7CService.Desk%40ru.nestle.com%7Cb4397e96b0ed4d41de8508dd1f3d892e%7C12a3af23a7694654847f958f3d479f4a%7C0%7C0%7C638701071341320637%7CUnknown%7CTWFpbGZsb3d8eyJFbXB0eU1hcGkiOnRydWUsIlYiOiIwLjAuMDAwMCIsIlAiOiJXaW4zMiIsIkFOIjoiTWFpbCIsIldUIjoyfQ%3D%3D%7C0%7C%7C%7C&amp;sdata=75JIvQ5VjDVWljZWag6nqVTl6jQmRU1a69mEz1a7Ijw%3D&amp;reserved=0" xr:uid="{F9CE9626-E882-4632-8F42-21189E39E532}"/>
-    <hyperlink ref="B13" r:id="rId12" display="https://elma.nestle.ru/_portal/service_desk/query_catalog(p:run/service_desk.applications/bms_roles;values=%7B%7D)" xr:uid="{ABA1F899-655B-4339-8720-89E53DDC3ED1}"/>
-    <hyperlink ref="B14" r:id="rId13" display="https://elma.nestle.ru/_portal/service_desk/query_catalog(p:run/service_desk.applications/directum_support;values=%7B%7D)" xr:uid="{C51EB03E-B549-436D-8DD8-52FFAA5CDC94}"/>
-    <hyperlink ref="B15" r:id="rId14" display="https://elma.nestle.ru/_portal/service_desk/query_catalog(p:run/service_desk.applications/req_elma;values=%7B%7D)" xr:uid="{AEBED057-815F-4681-B4B6-ADE1EF635355}"/>
-    <hyperlink ref="B16" r:id="rId15" display="https://elma.nestle.ru/_portal/service_desk/query_catalog(p:run/service_desk.applications/role_assignment_in_local_sap_prod_preprod;values=%7B%7D)" xr:uid="{78E6BFEB-632A-4E72-80DF-834E42B0BAC1}"/>
-    <hyperlink ref="B17" r:id="rId16" display="https://elma.nestle.ru/_portal/service_desk/query_catalog(p:run/service_desk.applications/reset_password_local_sap;values=%7B%7D)" xr:uid="{1222DA91-89D4-4FC8-87DB-FA8969E74BA2}"/>
-    <hyperlink ref="B18" r:id="rId17" display="https://elma.nestle.ru/_portal/service_desk/query_catalog(p:run/service_desk.applications/role_assignment_in_local_sap_preprod;values=%7B%7D)" xr:uid="{18903CB7-F83F-4D4E-BCF4-45AAF1F357F8}"/>
-    <hyperlink ref="B19" r:id="rId18" display="https://elma.nestle.ru/_portal/service_desk/query_catalog(p:run/service_desk.applications/reset_password_local_sap_non_prod;values=%7B%7D)" xr:uid="{C08F5CBC-C161-49AA-8076-37879964B50F}"/>
+    <hyperlink ref="B2" r:id="rId1" display="https://elma.nestle.ru/_portal/service_desk/query_catalog(p:run/service_desk.applications/equipment_issuance;values=%7B%7D)" xr:uid="{E0F770C9-4CFD-4AF5-81A4-2BBE388B5414}"/>
+    <hyperlink ref="B3" r:id="rId2" display="https://elma.nestle.ru/_portal/service_desk/query_catalog(p:run/service_desk.applications/mobile_service;values=%7B%7D)" xr:uid="{3285F7D5-B057-4BBE-8312-513A09028129}"/>
+    <hyperlink ref="B4" r:id="rId3" display="https://elma.nestle.ru/_portal/service_desk/query_catalog(p:run/service_desk.applications/software_maintenance;values=%7B%7D)" xr:uid="{F22114D6-7BE2-4BF3-861C-77D50FCFF03B}"/>
+    <hyperlink ref="B5" r:id="rId4" display="https://elma.nestle.ru/_portal/service_desk/query_catalog(p:run/service_desk.applications/installing_drivers_for_printers;values=%7B%7D)" xr:uid="{FFB30A37-182F-4E1A-B235-09CA9E9C8F41}"/>
+    <hyperlink ref="B6" r:id="rId5" display="https://elma.nestle.ru/_portal/service_desk/query_catalog(p:run/service_desk.applications/transfer_equipment;values=%7B%7D)" xr:uid="{15D5B86A-4043-41FA-8CE0-CC59B482F0DB}"/>
+    <hyperlink ref="B7" r:id="rId6" display="https://elma.nestle.ru/_portal/service_desk/query_catalog(p:run/service_desk.applications/IT_issue;values=%7B%7D)" xr:uid="{6F6335B1-71A8-4B34-912B-2EED075B03A0}"/>
+    <hyperlink ref="B8" r:id="rId7" display="https://elma.nestle.ru/_portal/service_desk/query_catalog(p:run/service_desk.applications/booking_equipment;values=%7B%7D)" xr:uid="{0B062787-85DD-4D31-9550-42E77050228C}"/>
+    <hyperlink ref="B9" r:id="rId8" display="https://elma.nestle.ru/_portal/service_desk/query_catalog(p:run/service_desk.applications/event_support;values=%7B%7D)" xr:uid="{88880065-36DF-4546-877E-617290DEDD2B}"/>
+    <hyperlink ref="B10" r:id="rId9" display="https://elma.nestle.ru/_portal/service_desk/query_catalog(p:run/service_desk.applications/Printer_maintenance;values=%7B%7D)" xr:uid="{5579DDD4-7906-4C5D-963D-1155D45A52F6}"/>
+    <hyperlink ref="B11" r:id="rId10" display="https://elma.nestle.ru/_portal/service_desk/query_catalog(p:run/service_desk.applications/consultant_plus;values=%7B%7D)" xr:uid="{1A3CD014-7891-48BF-A609-5021A066FD25}"/>
+    <hyperlink ref="B12" r:id="rId11" display="https://eur02.safelinks.protection.outlook.com/?url=https%3A%2F%2Felma.nestle.ru%2F_portal%2Fservice_desk%2Fquery_catalog(p%3Arun%2Fservice_desk.applications%2Frobots_report_an_issue%3Bvalues%3D%257B%257D)&amp;data=05%7C02%7CService.Desk%40ru.nestle.com%7Cb4397e96b0ed4d41de8508dd1f3d892e%7C12a3af23a7694654847f958f3d479f4a%7C0%7C0%7C638701071341320637%7CUnknown%7CTWFpbGZsb3d8eyJFbXB0eU1hcGkiOnRydWUsIlYiOiIwLjAuMDAwMCIsIlAiOiJXaW4zMiIsIkFOIjoiTWFpbCIsIldUIjoyfQ%3D%3D%7C0%7C%7C%7C&amp;sdata=75JIvQ5VjDVWljZWag6nqVTl6jQmRU1a69mEz1a7Ijw%3D&amp;reserved=0" xr:uid="{E7870727-4850-4941-B7B9-B5C098C76BCB}"/>
+    <hyperlink ref="B13" r:id="rId12" display="https://elma.nestle.ru/_portal/service_desk/query_catalog(p:run/service_desk.applications/bms_roles;values=%7B%7D)" xr:uid="{4497CE3F-58C0-43A0-B0BC-ABFA8834970D}"/>
+    <hyperlink ref="B14" r:id="rId13" display="https://elma.nestle.ru/_portal/service_desk/query_catalog(p:run/service_desk.applications/directum_support;values=%7B%7D)" xr:uid="{CDFBE5F9-2DB8-47D1-BF64-B27925D0A8B1}"/>
+    <hyperlink ref="B15" r:id="rId14" display="https://elma.nestle.ru/_portal/service_desk/query_catalog(p:run/service_desk.applications/req_elma;values=%7B%7D)" xr:uid="{13E24FCC-ABD2-453F-8D68-9692FC7B6910}"/>
+    <hyperlink ref="B16" r:id="rId15" display="https://elma.nestle.ru/_portal/service_desk/query_catalog(p:run/service_desk.applications/role_assignment_in_local_sap_prod_preprod;values=%7B%7D)" xr:uid="{EFD21501-D318-4883-97E4-D9B1E25DC685}"/>
+    <hyperlink ref="B17" r:id="rId16" display="https://elma.nestle.ru/_portal/service_desk/query_catalog(p:run/service_desk.applications/reset_password_local_sap;values=%7B%7D)" xr:uid="{EB1FD6B0-77E1-4C4C-8E74-0260B102322F}"/>
+    <hyperlink ref="B18" r:id="rId17" display="https://elma.nestle.ru/_portal/service_desk/query_catalog(p:run/service_desk.applications/role_assignment_in_local_sap_preprod;values=%7B%7D)" xr:uid="{7752035F-6D8A-418B-A079-B383D34E44A9}"/>
+    <hyperlink ref="B19" r:id="rId18" display="https://elma.nestle.ru/_portal/service_desk/query_catalog(p:run/service_desk.applications/reset_password_local_sap_non_prod;values=%7B%7D)" xr:uid="{F176A963-1647-48F5-ABDA-8A3732431156}"/>
+    <hyperlink ref="B23" r:id="rId19" display="https://elma.nestle.ru/_portal/service_desk/query_catalog(p:run/service_desk.applications/mailbox_creation_and_o365_license_change;values=%7B%7D)" xr:uid="{B56A2436-6C52-4E96-B76F-41B133881EF6}"/>
+    <hyperlink ref="C23" r:id="rId20" display="https://elma.nestle.ru/_portal/service_desk/query_catalog(p:run/service_desk.applications/mailbox_creation_and_o365_license_change;values=%7B%7D" xr:uid="{B70073C2-6D00-4730-A7B2-434473233B7A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId19"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId21"/>
 </worksheet>
 </file>
 
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{1ada0a2f-b917-4d51-b0d0-d418a10c8b23}" enabled="1" method="Standard" siteId="{12a3af23-a769-4654-847f-958f3d479f4a}" contentBits="0" removed="0"/>
+  <clbl:label id="{21be06aa-3a26-4c7d-8250-c00bd5d95b97}" enabled="1" method="Standard" siteId="{edf0de9d-7fa0-4684-ba48-b8e9ac9b8068}" contentBits="0" removed="0"/>
 </clbl:labelList>
 </file>
</xml_diff>